<commit_message>
Fin de la première journée
les maquettes ne sont pas encore disponible dans la docs
</commit_message>
<xml_diff>
--- a/docs/Planification.xlsx
+++ b/docs/Planification.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E898153A-BEE6-4C54-B6E1-4BAC163F7AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EA526C-DAC5-45FF-8535-DD6C94BCE148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="42960" yWindow="2865" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
-    <sheet name="Planning réel" sheetId="2" r:id="rId2"/>
+    <sheet name="Planning réel" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -250,7 +250,10 @@
     <t>Temps pour 1j de travail en heures</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Page détails d'un article</t>
+  </si>
+  <si>
+    <t>Ajout au panier depuis la page de détails d'un article</t>
   </si>
 </sst>
 </file>
@@ -925,6 +928,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -943,21 +964,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -967,14 +973,191 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="137">
+  <dxfs count="92">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1459,630 +1642,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
           <bgColor rgb="FFFBCFCF"/>
         </patternFill>
       </fill>
@@ -2617,10 +2176,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -2985,7 +2547,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="D16" s="22"/>
-      <c r="E16" s="51"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4">
         <v>0.10416666666666667</v>
       </c>
@@ -3002,7 +2564,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
@@ -3027,7 +2589,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>58</v>
       </c>
@@ -3052,7 +2614,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
         <v>34</v>
       </c>
@@ -3070,7 +2632,7 @@
       <c r="N19" s="26"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
@@ -3095,7 +2657,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19" t="s">
         <v>43</v>
       </c>
@@ -3113,7 +2675,7 @@
       <c r="N21" s="26"/>
       <c r="O21" s="21"/>
     </row>
-    <row r="22" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
@@ -3138,7 +2700,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
         <v>44</v>
       </c>
@@ -3156,7 +2718,7 @@
       <c r="N23" s="26"/>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -3180,11 +2742,8 @@
         <f>SUM(D24:N24)</f>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -3208,11 +2767,8 @@
         <f t="shared" ref="O25:O27" si="1">SUM(D25:N25)</f>
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
@@ -3236,11 +2792,8 @@
         <f t="shared" si="1"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>57</v>
       </c>
@@ -3264,11 +2817,8 @@
         <f t="shared" si="1"/>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="19" t="s">
         <v>45</v>
       </c>
@@ -3286,7 +2836,7 @@
       <c r="N28" s="26"/>
       <c r="O28" s="21"/>
     </row>
-    <row r="29" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>63</v>
       </c>
@@ -3310,11 +2860,8 @@
         <f t="shared" ref="O29:O30" si="2">SUM(D29:N29)</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
@@ -3338,11 +2885,8 @@
         <f t="shared" si="2"/>
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
         <v>46</v>
       </c>
@@ -3360,7 +2904,7 @@
       <c r="N31" s="26"/>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>59</v>
       </c>
@@ -3384,11 +2928,8 @@
         <f t="shared" ref="O32" si="3">SUM(D32:N32)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19" t="s">
         <v>47</v>
       </c>
@@ -3406,7 +2947,7 @@
       <c r="N33" s="26"/>
       <c r="O33" s="21"/>
     </row>
-    <row r="34" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>60</v>
       </c>
@@ -3430,11 +2971,8 @@
         <f t="shared" ref="O34" si="4">SUM(D34:N34)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P34" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
         <v>48</v>
       </c>
@@ -3452,7 +2990,7 @@
       <c r="N35" s="26"/>
       <c r="O35" s="21"/>
     </row>
-    <row r="36" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>61</v>
       </c>
@@ -3476,11 +3014,8 @@
         <f t="shared" ref="O36" si="5">SUM(D36:N36)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="P36" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
         <v>49</v>
       </c>
@@ -3498,7 +3033,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="21"/>
     </row>
-    <row r="38" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>62</v>
       </c>
@@ -3522,11 +3057,8 @@
         <f>SUM(D38:N38)</f>
         <v>0.10416666666666667</v>
       </c>
-      <c r="P38" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>37</v>
       </c>
@@ -3544,7 +3076,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="21"/>
     </row>
-    <row r="40" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
@@ -3568,11 +3100,8 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="P40" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="19" t="s">
         <v>35</v>
       </c>
@@ -3590,7 +3119,7 @@
       <c r="N41" s="26"/>
       <c r="O41" s="21"/>
     </row>
-    <row r="42" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>36</v>
       </c>
@@ -3618,11 +3147,8 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="P42" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="19" t="s">
         <v>24</v>
       </c>
@@ -3640,7 +3166,7 @@
       <c r="N43" s="26"/>
       <c r="O43" s="21"/>
     </row>
-    <row r="44" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>21</v>
       </c>
@@ -3685,7 +3211,7 @@
         <v>0.22916666666666669</v>
       </c>
     </row>
-    <row r="45" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>22</v>
       </c>
@@ -3718,7 +3244,7 @@
         <v>0.20833333333333331</v>
       </c>
     </row>
-    <row r="46" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3287,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="47" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
@@ -3786,7 +3312,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="19" t="s">
         <v>19</v>
       </c>
@@ -3887,51 +3413,51 @@
         <v>12</v>
       </c>
       <c r="C51" s="6">
-        <f>SUM(C3:C50)</f>
+        <f t="shared" ref="C51:N51" si="6">SUM(C3:C50)</f>
         <v>3.6666666666666661</v>
       </c>
       <c r="D51" s="5">
-        <f>SUM(D3:D50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333337</v>
       </c>
       <c r="E51" s="5">
-        <f>SUM(E3:E50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F51" s="5">
-        <f>SUM(F3:F50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G51" s="5">
-        <f>SUM(G3:G50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333326</v>
       </c>
       <c r="H51" s="5">
-        <f>SUM(H3:H50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I51" s="5">
-        <f>SUM(I3:I50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J51" s="5">
-        <f>SUM(J3:J50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333326</v>
       </c>
       <c r="K51" s="5">
-        <f>SUM(K3:K50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="L51" s="5">
-        <f>SUM(L3:L50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333326</v>
       </c>
       <c r="M51" s="5">
-        <f>SUM(M3:M50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="N51" s="5">
-        <f>SUM(N3:N50)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O51" s="6">
@@ -3986,17 +3512,17 @@
       <c r="O54" s="4"/>
     </row>
     <row r="55" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="47"/>
+      <c r="C55" s="42"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="48" t="s">
+      <c r="E55" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="51"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4009,16 +3535,16 @@
       <c r="B56" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="37">
         <v>3.6666666666666665</v>
       </c>
       <c r="D56" s="4"/>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="43">
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="37">
         <f>SUM(C4:C5,C7:C10)</f>
         <v>0.58333333333333337</v>
       </c>
@@ -4034,16 +3560,16 @@
       <c r="B57" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="45">
+      <c r="C57" s="39">
         <v>0.33333333333333331</v>
       </c>
       <c r="D57" s="4"/>
-      <c r="E57" s="39" t="s">
+      <c r="E57" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="44">
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="38">
         <f>SUM(C12:C14,C16:C18,C20,C22,C24:C27,C29:C30,C32,C34,C36,C38,C40,C42)</f>
         <v>1.5</v>
       </c>
@@ -4056,23 +3582,23 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E58" s="39" t="s">
+      <c r="E58" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="44">
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="38">
         <f>SUM(C44:C47)</f>
         <v>1.25</v>
       </c>
     </row>
     <row r="59" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E59" s="41" t="s">
+      <c r="E59" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="45">
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="39">
         <f>SUM(C49:C50)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -4088,177 +3614,237 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="61" priority="38">
+    <cfRule type="expression" dxfId="91" priority="51">
       <formula xml:space="preserve"> $C$51&lt;&gt;$C$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="60" priority="37">
+    <cfRule type="expression" dxfId="90" priority="50">
       <formula xml:space="preserve"> $D$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:N50">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="89" priority="52">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="58" priority="36">
+    <cfRule type="expression" dxfId="88" priority="49">
       <formula xml:space="preserve"> $E$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="expression" dxfId="57" priority="35">
+    <cfRule type="expression" dxfId="87" priority="48">
       <formula xml:space="preserve"> $F$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="56" priority="34">
+    <cfRule type="expression" dxfId="86" priority="47">
       <formula xml:space="preserve"> $G$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="55" priority="33">
+    <cfRule type="expression" dxfId="85" priority="46">
       <formula xml:space="preserve"> $H$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="54" priority="32">
+    <cfRule type="expression" dxfId="84" priority="45">
       <formula xml:space="preserve"> $I$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51">
-    <cfRule type="expression" dxfId="53" priority="31">
+    <cfRule type="expression" dxfId="83" priority="44">
       <formula xml:space="preserve"> $J$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51">
-    <cfRule type="expression" dxfId="52" priority="30">
+    <cfRule type="expression" dxfId="82" priority="43">
       <formula xml:space="preserve"> $K$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51">
-    <cfRule type="expression" dxfId="51" priority="29">
+    <cfRule type="expression" dxfId="81" priority="42">
       <formula xml:space="preserve"> $L$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M51">
-    <cfRule type="expression" dxfId="50" priority="28">
+    <cfRule type="expression" dxfId="80" priority="41">
       <formula xml:space="preserve"> $M$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51">
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="79" priority="40">
       <formula xml:space="preserve"> $N$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="expression" dxfId="48" priority="15">
+    <cfRule type="expression" dxfId="78" priority="28">
       <formula>$O$4&lt;&gt;$C$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="47" priority="16">
+    <cfRule type="expression" dxfId="77" priority="29">
       <formula>$O$5&lt;&gt;$C$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="46" priority="17">
+    <cfRule type="expression" dxfId="76" priority="30">
       <formula>$O$7&lt;&gt;$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="expression" dxfId="45" priority="18">
+    <cfRule type="expression" dxfId="75" priority="31">
       <formula>$O$8&lt;&gt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="expression" dxfId="44" priority="21">
+    <cfRule type="expression" dxfId="74" priority="34">
       <formula>$O$9&lt;&gt;$C$9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O10">
+    <cfRule type="expression" dxfId="73" priority="22">
+      <formula>$O$10&lt;&gt;$C$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O12">
+    <cfRule type="expression" dxfId="72" priority="21">
+      <formula>$O$12&lt;&gt;$C$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O13">
+    <cfRule type="expression" dxfId="71" priority="20">
+      <formula>$O$13&lt;&gt;$C$13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14">
+    <cfRule type="expression" dxfId="70" priority="19">
+      <formula>$O$14&lt;&gt;$C$14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
+    <cfRule type="expression" dxfId="69" priority="18">
+      <formula>$O$16&lt;&gt;$C$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="expression" dxfId="68" priority="17">
+      <formula>$O$17&lt;&gt;$C$17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
+    <cfRule type="expression" dxfId="67" priority="16">
+      <formula>$O$18&lt;&gt;$C$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20">
+    <cfRule type="expression" dxfId="66" priority="15">
+      <formula>$O$20&lt;&gt;$C$20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22">
+    <cfRule type="expression" dxfId="65" priority="14">
+      <formula>$O$22&lt;&gt;$C$22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O24">
+    <cfRule type="expression" dxfId="64" priority="13">
+      <formula>$O$24&lt;&gt;$C$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O25">
+    <cfRule type="expression" dxfId="63" priority="12">
+      <formula>$O$25&lt;&gt;$C$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26">
+    <cfRule type="expression" dxfId="62" priority="11">
+      <formula>$O$26&lt;&gt;$C$26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27">
+    <cfRule type="expression" dxfId="61" priority="10">
+      <formula>$O$27&lt;&gt;$C$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O29">
+    <cfRule type="expression" dxfId="60" priority="9">
+      <formula>$O$29&lt;&gt;$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O30">
+    <cfRule type="expression" dxfId="59" priority="8">
+      <formula>$O$30&lt;&gt;$C$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O32">
+    <cfRule type="expression" dxfId="58" priority="7">
+      <formula>$O$32&lt;&gt;$C$32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34">
+    <cfRule type="expression" dxfId="57" priority="6">
+      <formula>$O$34&lt;&gt;$C$34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O36">
+    <cfRule type="expression" dxfId="56" priority="5">
+      <formula>$O$36&lt;&gt;$C$36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O38">
+    <cfRule type="expression" dxfId="55" priority="4">
+      <formula>$O$38&lt;&gt;$C$38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O40">
+    <cfRule type="expression" dxfId="54" priority="3">
+      <formula>$O$40&lt;&gt;$C$40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O42">
+    <cfRule type="expression" dxfId="53" priority="1">
+      <formula>$O$42&lt;&gt;$C$42</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O44">
-    <cfRule type="expression" dxfId="43" priority="14">
+    <cfRule type="expression" dxfId="52" priority="27">
       <formula>$O$44&lt;&gt;$C$44</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O45">
-    <cfRule type="expression" dxfId="42" priority="13">
+    <cfRule type="expression" dxfId="51" priority="26">
       <formula>$O$45&lt;&gt;$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O46">
-    <cfRule type="expression" dxfId="41" priority="12">
+    <cfRule type="expression" dxfId="50" priority="25">
       <formula>$O$46&lt;&gt;$C$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O47">
-    <cfRule type="expression" dxfId="40" priority="11">
+    <cfRule type="expression" dxfId="49" priority="24">
       <formula>$O$47&lt;&gt;$C$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49">
-    <cfRule type="expression" dxfId="39" priority="22">
+    <cfRule type="expression" dxfId="48" priority="35">
       <formula>$O$49&lt;&gt;$C$49</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50">
-    <cfRule type="expression" dxfId="38" priority="23">
+    <cfRule type="expression" dxfId="47" priority="36">
       <formula xml:space="preserve"> $O$50&lt;&gt;$C$50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O51">
-    <cfRule type="expression" dxfId="37" priority="25">
+    <cfRule type="expression" dxfId="46" priority="38">
       <formula xml:space="preserve"> $O$51&lt;&gt;$C$56</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
-    <cfRule type="expression" dxfId="36" priority="9">
-      <formula>$O$10&lt;&gt;$C$10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O12">
-    <cfRule type="expression" dxfId="35" priority="8">
-      <formula>$O$12&lt;&gt;$C$12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O13">
-    <cfRule type="expression" dxfId="34" priority="7">
-      <formula>$O$13&lt;&gt;$C$13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O14">
-    <cfRule type="expression" dxfId="33" priority="6">
-      <formula>$O$14&lt;&gt;$C$14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O16">
-    <cfRule type="expression" dxfId="32" priority="5">
-      <formula>$O$16&lt;&gt;$C$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17">
-    <cfRule type="expression" dxfId="31" priority="4">
-      <formula>$O$17&lt;&gt;$C$17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="expression" dxfId="30" priority="3">
-      <formula>$O$18&lt;&gt;$C$18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O20">
-    <cfRule type="expression" dxfId="29" priority="2">
-      <formula>$O$20&lt;&gt;$C$20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O22">
-    <cfRule type="expression" dxfId="28" priority="1">
-      <formula>$O$22&lt;&gt;$C$22</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="35" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="O44:O47 O49:O50 O4:O5 O7:O10 O12:O27 O29:O30 O32:O42" formulaRange="1"/>
   </ignoredErrors>
@@ -4266,11 +3852,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366A89D5-D9FA-490B-9591-C0459C941711}">
-  <dimension ref="B1:P59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AB6151-ACBB-4F8A-A877-2979D67AF922}">
+  <dimension ref="B1:P61"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -4353,7 +3939,9 @@
       <c r="C4" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="22">
+        <v>3.4722222222222224E-2</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -4366,7 +3954,7 @@
       <c r="N4" s="23"/>
       <c r="O4" s="9">
         <f t="shared" ref="O4:O50" si="0">SUM(D4:N4)</f>
-        <v>0</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4376,7 +3964,9 @@
       <c r="C5" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="22">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -4389,7 +3979,7 @@
       <c r="N5" s="23"/>
       <c r="O5" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4417,7 +4007,9 @@
       <c r="C7" s="7">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="22">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -4430,7 +4022,7 @@
       <c r="N7" s="23"/>
       <c r="O7" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4440,7 +4032,9 @@
       <c r="C8" s="7">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="22">
+        <v>9.375E-2</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -4453,7 +4047,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4615,7 +4209,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="D16" s="22"/>
-      <c r="E16" s="51"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -4719,7 +4313,7 @@
     </row>
     <row r="21" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="24"/>
@@ -5055,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
         <v>49</v>
       </c>
@@ -5073,7 +4667,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="21"/>
     </row>
-    <row r="38" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>62</v>
       </c>
@@ -5096,7 +4690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
         <v>37</v>
       </c>
@@ -5114,7 +4708,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="21"/>
     </row>
-    <row r="40" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
@@ -5137,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="19" t="s">
         <v>35</v>
       </c>
@@ -5155,12 +4749,12 @@
       <c r="N41" s="26"/>
       <c r="O41" s="21"/>
     </row>
-    <row r="42" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="7">
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="4"/>
@@ -5178,7 +4772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="19" t="s">
         <v>24</v>
       </c>
@@ -5196,14 +4790,16 @@
       <c r="N43" s="26"/>
       <c r="O43" s="21"/>
     </row>
-    <row r="44" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C44" s="7">
         <v>0.22916666666666666</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="22">
+        <v>3.4722222222222224E-2</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -5216,10 +4812,10 @@
       <c r="N44" s="23"/>
       <c r="O44" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3.4722222222222224E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>22</v>
       </c>
@@ -5242,14 +4838,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="7">
         <v>0.75</v>
       </c>
-      <c r="D46" s="22"/>
+      <c r="D46" s="22">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -5262,10 +4860,10 @@
       <c r="N46" s="23"/>
       <c r="O46" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
@@ -5288,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="19" t="s">
         <v>19</v>
       </c>
@@ -5306,12 +4904,12 @@
       <c r="N48" s="26"/>
       <c r="O48" s="21"/>
     </row>
-    <row r="49" spans="2:16" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="7">
-        <v>0.20833333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="4"/>
@@ -5329,12 +4927,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:16" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="8">
-        <v>0.20833333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D50" s="27"/>
       <c r="E50" s="28"/>
@@ -5352,65 +4950,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:16" s="1" customFormat="1" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="6">
-        <f>SUM(C3:C50)</f>
-        <v>3.6666666666666665</v>
+        <f t="shared" ref="C51:N51" si="6">SUM(C3:C50)</f>
+        <v>3.6666666666666661</v>
       </c>
       <c r="D51" s="5">
-        <f>SUM(D3:D50)</f>
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E51" s="5">
-        <f>SUM(E3:E50)</f>
+      <c r="F51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F51" s="5">
-        <f>SUM(F3:F50)</f>
+      <c r="G51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G51" s="5">
-        <f>SUM(G3:G50)</f>
+      <c r="H51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H51" s="5">
-        <f>SUM(H3:H50)</f>
+      <c r="I51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I51" s="5">
-        <f>SUM(I3:I50)</f>
+      <c r="J51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J51" s="5">
-        <f>SUM(J3:J50)</f>
+      <c r="K51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K51" s="5">
-        <f>SUM(K3:K50)</f>
+      <c r="L51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L51" s="5">
-        <f>SUM(L3:L50)</f>
+      <c r="M51" s="5">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M51" s="5">
-        <f>SUM(M3:M50)</f>
-        <v>0</v>
-      </c>
       <c r="N51" s="5">
-        <f>SUM(N3:N50)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O51" s="6">
         <f>SUM(D51:N51)</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="2:16" s="1" customFormat="1" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -5425,7 +5023,7 @@
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
     </row>
-    <row r="53" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -5440,7 +5038,7 @@
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
     </row>
-    <row r="54" spans="2:16" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -5455,18 +5053,18 @@
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
     </row>
-    <row r="55" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="46" t="s">
+    <row r="55" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="47"/>
+      <c r="C55" s="42"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="48" t="s">
+      <c r="E55" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="51"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -5475,20 +5073,20 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="37">
         <v>3.6666666666666665</v>
       </c>
       <c r="D56" s="4"/>
-      <c r="E56" s="37" t="s">
+      <c r="E56" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="43">
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="37">
         <f>SUM(C4:C5,C7:C10)</f>
         <v>0.58333333333333337</v>
       </c>
@@ -5500,22 +5098,22 @@
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
     </row>
-    <row r="57" spans="2:16" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="45">
+      <c r="C57" s="39">
         <v>0.33333333333333331</v>
       </c>
       <c r="D57" s="4"/>
-      <c r="E57" s="39" t="s">
+      <c r="E57" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="44">
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="38">
         <f>SUM(C12:C14,C16:C18,C20,C22,C24:C27,C29:C30,C32,C34,C36,C38,C40,C42)</f>
-        <v>1.4166666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -5525,163 +5123,276 @@
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E58" s="39" t="s">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E58" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="44">
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="38">
         <f>SUM(C44:C47)</f>
         <v>1.25</v>
       </c>
     </row>
-    <row r="59" spans="2:16" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E59" s="41" t="s">
+    <row r="59" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E59" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="45">
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="39">
         <f>SUM(C49:C50)</f>
-        <v>0.41666666666666669</v>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="E59:G59"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="E55:H55"/>
     <mergeCell ref="E56:G56"/>
     <mergeCell ref="E57:G57"/>
     <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
   </mergeCells>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="136" priority="24">
+    <cfRule type="expression" dxfId="45" priority="45">
       <formula xml:space="preserve"> $C$51&lt;&gt;$C$56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="135" priority="23">
+    <cfRule type="expression" dxfId="44" priority="44">
       <formula xml:space="preserve"> $D$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:N50">
-    <cfRule type="notContainsBlanks" dxfId="134" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="46">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="133" priority="22">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula xml:space="preserve"> $E$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="expression" dxfId="132" priority="21">
+    <cfRule type="expression" dxfId="41" priority="42">
       <formula xml:space="preserve"> $F$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="131" priority="20">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula xml:space="preserve"> $G$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="130" priority="19">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula xml:space="preserve"> $H$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="129" priority="18">
+    <cfRule type="expression" dxfId="38" priority="39">
       <formula xml:space="preserve"> $I$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51">
-    <cfRule type="expression" dxfId="128" priority="17">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula xml:space="preserve"> $J$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51">
-    <cfRule type="expression" dxfId="127" priority="16">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula xml:space="preserve"> $K$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51">
-    <cfRule type="expression" dxfId="126" priority="15">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula xml:space="preserve"> $L$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M51">
-    <cfRule type="expression" dxfId="125" priority="14">
+    <cfRule type="expression" dxfId="34" priority="35">
       <formula xml:space="preserve"> $M$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51">
-    <cfRule type="expression" dxfId="124" priority="13">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula xml:space="preserve"> $N$51&lt;&gt;$C$57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="expression" dxfId="123" priority="5">
+    <cfRule type="expression" dxfId="32" priority="26">
       <formula>$O$4&lt;&gt;$C$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="122" priority="6">
+    <cfRule type="expression" dxfId="31" priority="27">
       <formula>$O$5&lt;&gt;$C$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="expression" dxfId="121" priority="7">
+    <cfRule type="expression" dxfId="30" priority="28">
       <formula>$O$7&lt;&gt;$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="expression" dxfId="120" priority="8">
+    <cfRule type="expression" dxfId="29" priority="29">
       <formula>$O$8&lt;&gt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9:O10">
-    <cfRule type="expression" dxfId="119" priority="9">
+  <conditionalFormatting sqref="O9">
+    <cfRule type="expression" dxfId="28" priority="30">
       <formula>$O$9&lt;&gt;$C$9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O10">
+    <cfRule type="expression" dxfId="27" priority="21">
+      <formula>$O$10&lt;&gt;$C$10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O12">
+    <cfRule type="expression" dxfId="26" priority="20">
+      <formula>$O$12&lt;&gt;$C$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O13">
+    <cfRule type="expression" dxfId="25" priority="19">
+      <formula>$O$13&lt;&gt;$C$13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14">
+    <cfRule type="expression" dxfId="24" priority="18">
+      <formula>$O$14&lt;&gt;$C$14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>$O$16&lt;&gt;$C$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="expression" dxfId="22" priority="16">
+      <formula>$O$17&lt;&gt;$C$17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
+    <cfRule type="expression" dxfId="21" priority="15">
+      <formula>$O$18&lt;&gt;$C$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20">
+    <cfRule type="expression" dxfId="20" priority="14">
+      <formula>$O$20&lt;&gt;$C$20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22">
+    <cfRule type="expression" dxfId="19" priority="13">
+      <formula>$O$22&lt;&gt;$C$22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O24">
+    <cfRule type="expression" dxfId="18" priority="12">
+      <formula>$O$24&lt;&gt;$C$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O25">
+    <cfRule type="expression" dxfId="17" priority="11">
+      <formula>$O$25&lt;&gt;$C$25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O26">
+    <cfRule type="expression" dxfId="16" priority="10">
+      <formula>$O$26&lt;&gt;$C$26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>$O$27&lt;&gt;$C$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O29">
+    <cfRule type="expression" dxfId="14" priority="8">
+      <formula>$O$29&lt;&gt;$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O30">
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>$O$30&lt;&gt;$C$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O32">
+    <cfRule type="expression" dxfId="12" priority="6">
+      <formula>$O$32&lt;&gt;$C$32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34">
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>$O$34&lt;&gt;$C$34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O36">
+    <cfRule type="expression" dxfId="10" priority="4">
+      <formula>$O$36&lt;&gt;$C$36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O38">
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>$O$38&lt;&gt;$C$38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O40">
+    <cfRule type="expression" dxfId="8" priority="2">
+      <formula>$O$40&lt;&gt;$C$40</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O42">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>$O$42&lt;&gt;$C$42</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O44">
-    <cfRule type="expression" dxfId="118" priority="4">
+    <cfRule type="expression" dxfId="6" priority="25">
       <formula>$O$44&lt;&gt;$C$44</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O45">
-    <cfRule type="expression" dxfId="117" priority="3">
+    <cfRule type="expression" dxfId="5" priority="24">
       <formula>$O$45&lt;&gt;$C$45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O46">
-    <cfRule type="expression" dxfId="116" priority="2">
+    <cfRule type="expression" dxfId="4" priority="23">
       <formula>$O$46&lt;&gt;$C$46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O47">
-    <cfRule type="expression" dxfId="115" priority="1">
+    <cfRule type="expression" dxfId="3" priority="22">
       <formula>$O$47&lt;&gt;$C$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49">
-    <cfRule type="expression" dxfId="114" priority="10">
+    <cfRule type="expression" dxfId="2" priority="31">
       <formula>$O$49&lt;&gt;$C$49</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50">
-    <cfRule type="expression" dxfId="113" priority="11">
+    <cfRule type="expression" dxfId="1" priority="32">
       <formula xml:space="preserve"> $O$50&lt;&gt;$C$50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O51">
-    <cfRule type="expression" dxfId="112" priority="12">
+    <cfRule type="expression" dxfId="0" priority="33">
       <formula xml:space="preserve"> $O$51&lt;&gt;$C$56</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="O4:O50" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout des maquettes et du MCD, Réalisation cas de tests
Avancement dans la doc technique
</commit_message>
<xml_diff>
--- a/docs/Planification.xlsx
+++ b/docs/Planification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EA526C-DAC5-45FF-8535-DD6C94BCE148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA013641-FF6B-4ACD-A6C0-C9C8647C3E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="42960" yWindow="2865" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -254,6 +254,49 @@
   </si>
   <si>
     <t>Ajout au panier depuis la page de détails d'un article</t>
+  </si>
+  <si>
+    <t>Temps
+prévisionnel</t>
+  </si>
+  <si>
+    <t>Temps réel effectué (tâches)</t>
+  </si>
+  <si>
+    <t>Page de recherche</t>
+  </si>
+  <si>
+    <t>Afficher les 10 articles mis à la une</t>
+  </si>
+  <si>
+    <t>Afficher les articles selon le filtre</t>
+  </si>
+  <si>
+    <t>Implémentation des données nécessaires (villes Suisse)</t>
+  </si>
+  <si>
+    <t>Afficher les informations de l'article</t>
+  </si>
+  <si>
+    <t>Ajouter l'article au panier</t>
+  </si>
+  <si>
+    <t>Afficher le nombre total d'articles et le prix total TTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier la quantité de chaques articles </t>
+  </si>
+  <si>
+    <t>Afficher les articles dans le panier</t>
+  </si>
+  <si>
+    <t>Afficher les informations de la page</t>
+  </si>
+  <si>
+    <t>Réalisation du backlog (doc)</t>
+  </si>
+  <si>
+    <t>Réalisation des scénarios de tests (doc)</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1020,465 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="138">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFBCFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2181,7 +2682,7 @@
   </sheetPr>
   <dimension ref="B1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -3853,10 +4354,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AB6151-ACBB-4F8A-A877-2979D67AF922}">
-  <dimension ref="B1:P61"/>
+  <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -3864,7 +4365,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="77.85546875" style="1" customWidth="1"/>
     <col min="3" max="14" width="20.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="20.7109375" style="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -3875,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>1</v>
@@ -3911,7 +4412,7 @@
         <v>11</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -3953,7 +4454,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="23"/>
       <c r="O4" s="9">
-        <f t="shared" ref="O4:O50" si="0">SUM(D4:N4)</f>
+        <f t="shared" ref="O4:O53" si="0">SUM(D4:N4)</f>
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
@@ -4035,7 +4536,9 @@
       <c r="D8" s="22">
         <v>9.375E-2</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>6.25E-2</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -4047,7 +4550,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="9">
         <f t="shared" si="0"/>
-        <v>9.375E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4058,7 +4561,9 @@
         <v>9.7222222222222224E-2</v>
       </c>
       <c r="D9" s="22"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -4070,18 +4575,20 @@
       <c r="N9" s="23"/>
       <c r="O9" s="9">
         <f t="shared" si="0"/>
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0.125</v>
-      </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>7.2916666666666671E-2</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -4091,58 +4598,60 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="23"/>
-      <c r="O10" s="34">
+      <c r="O10" s="15">
         <f>SUM(D10:N10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+        <v>7.2916666666666671E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="34">
+        <f>SUM(D11:N11)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="21"/>
-    </row>
-    <row r="12" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="C12" s="20"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="7">
         <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="7">
-        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="4"/>
@@ -4155,61 +4664,61 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="23"/>
-      <c r="O13" s="33">
-        <f>SUM(D13:N13)</f>
+      <c r="O13" s="15">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="21"/>
+    </row>
+    <row r="15" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="33">
+        <f>SUM(D15:N15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C16" s="7">
         <v>0.1111111111111111</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="33">
-        <f>SUM(D14:N14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="21"/>
-    </row>
-    <row r="16" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0.10416666666666667</v>
-      </c>
       <c r="D16" s="22"/>
-      <c r="E16" s="40"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -4219,43 +4728,38 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="23"/>
-      <c r="O16" s="9">
-        <f t="shared" si="0"/>
+      <c r="O16" s="33">
+        <f>SUM(D16:N16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="9">
-        <f>SUM(D17:N17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="21"/>
+    </row>
+    <row r="18" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7">
-        <v>1.3888888888888888E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D18" s="22"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -4266,34 +4770,39 @@
       <c r="M18" s="4"/>
       <c r="N18" s="23"/>
       <c r="O18" s="9">
-        <f>SUM(D18:N18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="21"/>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="9">
+        <f>SUM(D19:N19)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="C20" s="7">
-        <v>4.1666666666666664E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="4"/>
@@ -4307,13 +4816,13 @@
       <c r="M20" s="4"/>
       <c r="N20" s="23"/>
       <c r="O20" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D20:N20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="24"/>
@@ -4331,7 +4840,7 @@
     </row>
     <row r="22" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7">
         <v>4.1666666666666664E-2</v>
@@ -4348,13 +4857,13 @@
       <c r="M22" s="4"/>
       <c r="N22" s="23"/>
       <c r="O22" s="9">
-        <f>SUM(D22:N22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="24"/>
@@ -4372,10 +4881,10 @@
     </row>
     <row r="24" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="C24" s="7">
-        <v>2.7777777777777776E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="4"/>
@@ -4393,12 +4902,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C25" s="7">
-        <v>1.3888888888888888E-2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="4"/>
@@ -4411,40 +4920,32 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="23"/>
-      <c r="O25" s="9">
-        <f t="shared" ref="O25:O27" si="1">SUM(D25:N25)</f>
-        <v>0</v>
-      </c>
+      <c r="O25" s="33"/>
     </row>
     <row r="26" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="7">
+      <c r="B26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="21"/>
+    </row>
+    <row r="27" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="7">
         <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="4"/>
@@ -4458,34 +4959,39 @@
       <c r="M27" s="4"/>
       <c r="N27" s="23"/>
       <c r="O27" s="9">
-        <f t="shared" si="1"/>
+        <f>SUM(D27:N27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="21"/>
+      <c r="B28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="9">
+        <f t="shared" ref="O28:O30" si="1">SUM(D28:N28)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="C29" s="7">
-        <v>2.0833333333333332E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="4"/>
@@ -4499,16 +5005,16 @@
       <c r="M29" s="4"/>
       <c r="N29" s="23"/>
       <c r="O29" s="9">
-        <f t="shared" ref="O29:O30" si="2">SUM(D29:N29)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C30" s="7">
-        <v>1.3888888888888888E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="4"/>
@@ -4521,14 +5027,14 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="23"/>
-      <c r="O30" s="15">
-        <f t="shared" si="2"/>
+      <c r="O30" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="24"/>
@@ -4544,12 +5050,12 @@
       <c r="N31" s="26"/>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C32" s="7">
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="4"/>
@@ -4563,264 +5069,262 @@
       <c r="M32" s="4"/>
       <c r="N32" s="23"/>
       <c r="O32" s="9">
-        <f t="shared" ref="O32" si="3">SUM(D32:N32)</f>
+        <f t="shared" ref="O32:O33" si="2">SUM(D32:N32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
+    <row r="33" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="21"/>
+    </row>
+    <row r="35" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="9">
+        <f t="shared" ref="O35" si="3">SUM(D35:N35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="21"/>
-    </row>
-    <row r="34" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="21"/>
+    </row>
+    <row r="37" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C37" s="7">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="9">
-        <f t="shared" ref="O34" si="4">SUM(D34:N34)</f>
+      <c r="D37" s="22"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="9">
+        <f t="shared" ref="O37" si="4">SUM(D37:N37)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
+    <row r="38" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="21"/>
-    </row>
-    <row r="36" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
+      <c r="C38" s="20"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="21"/>
+    </row>
+    <row r="39" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C39" s="7">
         <v>6.25E-2</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="9">
-        <f t="shared" ref="O36" si="5">SUM(D36:N36)</f>
+      <c r="D39" s="22"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="9">
+        <f t="shared" ref="O39" si="5">SUM(D39:N39)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
+    <row r="40" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="21"/>
-    </row>
-    <row r="38" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="s">
+      <c r="C40" s="20"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="21"/>
+    </row>
+    <row r="41" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C41" s="7">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="9">
-        <f>SUM(D38:N38)</f>
+      <c r="D41" s="22"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="9">
+        <f>SUM(D41:N41)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="19" t="s">
+    <row r="42" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="21"/>
-    </row>
-    <row r="40" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
+      <c r="C42" s="20"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C43" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D40" s="22"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="9">
+      <c r="D43" s="22"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+    <row r="44" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="21"/>
-    </row>
-    <row r="42" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
+      <c r="C44" s="20"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="21"/>
+    </row>
+    <row r="45" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C45" s="7">
         <v>0.5</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="21"/>
-    </row>
-    <row r="44" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="7">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="D44" s="22">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="9">
-        <f t="shared" si="0"/>
-        <v>3.4722222222222224E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="7">
-        <v>0.20833333333333334</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="4"/>
@@ -4833,45 +5337,42 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
       <c r="N45" s="23"/>
-      <c r="O45" s="9">
+      <c r="O45" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="D46" s="22">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="9">
-        <f t="shared" si="0"/>
-        <v>2.7777777777777776E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="21"/>
+    </row>
+    <row r="47" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C47" s="7">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="4"/>
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D47" s="22">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -4881,39 +5382,50 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="23"/>
-      <c r="O47" s="15">
+      <c r="O47" s="9">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="21"/>
-    </row>
     <row r="49" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C49" s="7">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="D49" s="22">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F49" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
@@ -4924,93 +5436,58 @@
       <c r="N49" s="23"/>
       <c r="O49" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2361111111111111</v>
       </c>
     </row>
     <row r="50" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="9">
+      <c r="B50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D50" s="22"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="6">
-        <f t="shared" ref="C51:N51" si="6">SUM(C3:C50)</f>
-        <v>3.6666666666666661</v>
-      </c>
-      <c r="D51" s="5">
-        <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O51" s="6">
-        <f>SUM(D51:N51)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P51" s="4"/>
-    </row>
-    <row r="52" spans="2:16" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
+    <row r="51" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="20"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="21"/>
+    </row>
+    <row r="52" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D52" s="22"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -5020,51 +5497,100 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-    </row>
-    <row r="54" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-    </row>
-    <row r="55" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="42"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D53" s="27"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="29"/>
+      <c r="O53" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="6">
+        <f t="shared" ref="C54:N54" si="6">SUM(C3:C53)</f>
+        <v>3.6666666666666661</v>
+      </c>
+      <c r="D54" s="5">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E54" s="5">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="F54" s="5">
+        <f t="shared" si="6"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O54" s="6">
+        <f>SUM(D54:N54)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="P54" s="4"/>
+    </row>
+    <row r="55" spans="2:16" ht="20.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="51"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -5073,23 +5599,13 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="37">
-        <v>3.6666666666666665</v>
-      </c>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="37">
-        <f>SUM(C4:C5,C7:C10)</f>
-        <v>0.58333333333333337</v>
-      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -5098,23 +5614,13 @@
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
     </row>
-    <row r="57" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="39">
-        <v>0.33333333333333331</v>
-      </c>
+    <row r="57" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="F57" s="46"/>
-      <c r="G57" s="46"/>
-      <c r="H57" s="38">
-        <f>SUM(C12:C14,C16:C18,C20,C22,C24:C27,C29:C30,C32,C34,C36,C38,C40,C42)</f>
-        <v>1.5</v>
-      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -5123,105 +5629,175 @@
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E58" s="45" t="s">
+    <row r="58" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="42"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+    </row>
+    <row r="59" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="37">
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="37">
+        <f>SUM(C4:C5,C7:C11)</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+    </row>
+    <row r="60" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="39">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="38">
+        <f>SUM(C13:C16,C18:C20,C22,C24,C27:C30,C32:C33,C35,C37,C39,C41,C43,C45)</f>
+        <v>1.5</v>
+      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E61" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="46"/>
-      <c r="G58" s="46"/>
-      <c r="H58" s="38">
-        <f>SUM(C44:C47)</f>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="38">
+        <f>SUM(C47:C50)</f>
         <v>1.25</v>
       </c>
     </row>
-    <row r="59" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E59" s="47" t="s">
+    <row r="62" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="39">
-        <f>SUM(C49:C50)</f>
+      <c r="F62" s="48"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="39">
+        <f>SUM(C52:C53)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="E58:H58"/>
     <mergeCell ref="E59:G59"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="E55:H55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
   </mergeCells>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C54">
     <cfRule type="expression" dxfId="45" priority="45">
-      <formula xml:space="preserve"> $C$51&lt;&gt;$C$56</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
+      <formula xml:space="preserve"> $C$54&lt;&gt;$C$59</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
     <cfRule type="expression" dxfId="44" priority="44">
-      <formula xml:space="preserve"> $D$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:N50">
+      <formula xml:space="preserve"> $D$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:N53">
     <cfRule type="notContainsBlanks" dxfId="43" priority="46">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E54">
     <cfRule type="expression" dxfId="42" priority="43">
-      <formula xml:space="preserve"> $E$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
+      <formula xml:space="preserve"> $E$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F54">
     <cfRule type="expression" dxfId="41" priority="42">
-      <formula xml:space="preserve"> $F$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
+      <formula xml:space="preserve"> $F$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G54">
     <cfRule type="expression" dxfId="40" priority="41">
-      <formula xml:space="preserve"> $G$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
+      <formula xml:space="preserve"> $G$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
     <cfRule type="expression" dxfId="39" priority="40">
-      <formula xml:space="preserve"> $H$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
+      <formula xml:space="preserve"> $H$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54">
     <cfRule type="expression" dxfId="38" priority="39">
-      <formula xml:space="preserve"> $I$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J51">
+      <formula xml:space="preserve"> $I$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J54">
     <cfRule type="expression" dxfId="37" priority="38">
-      <formula xml:space="preserve"> $J$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K51">
+      <formula xml:space="preserve"> $J$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K54">
     <cfRule type="expression" dxfId="36" priority="37">
-      <formula xml:space="preserve"> $K$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
+      <formula xml:space="preserve"> $K$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L54">
     <cfRule type="expression" dxfId="35" priority="36">
-      <formula xml:space="preserve"> $L$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M51">
+      <formula xml:space="preserve"> $L$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M54">
     <cfRule type="expression" dxfId="34" priority="35">
-      <formula xml:space="preserve"> $M$51&lt;&gt;$C$57</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N51">
+      <formula xml:space="preserve"> $M$54&lt;&gt;$C$60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N54">
     <cfRule type="expression" dxfId="33" priority="34">
-      <formula xml:space="preserve"> $N$51&lt;&gt;$C$57</formula>
+      <formula xml:space="preserve"> $N$54&lt;&gt;$C$60</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
@@ -5244,155 +5820,155 @@
       <formula>$O$8&lt;&gt;$C$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9">
+  <conditionalFormatting sqref="O9:O10">
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>$O$9&lt;&gt;$C$9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
+  <conditionalFormatting sqref="O11">
     <cfRule type="expression" dxfId="27" priority="21">
-      <formula>$O$10&lt;&gt;$C$10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O12">
+      <formula>$O$11&lt;&gt;$C$11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O13">
     <cfRule type="expression" dxfId="26" priority="20">
-      <formula>$O$12&lt;&gt;$C$12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O13">
+      <formula>$O$13&lt;&gt;$C$13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15">
     <cfRule type="expression" dxfId="25" priority="19">
-      <formula>$O$13&lt;&gt;$C$13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O14">
+      <formula>$O$15&lt;&gt;$C$15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
     <cfRule type="expression" dxfId="24" priority="18">
-      <formula>$O$14&lt;&gt;$C$14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O16">
+      <formula>$O$16&lt;&gt;$C$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
     <cfRule type="expression" dxfId="23" priority="17">
-      <formula>$O$16&lt;&gt;$C$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17">
+      <formula>$O$18&lt;&gt;$C$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19">
     <cfRule type="expression" dxfId="22" priority="16">
-      <formula>$O$17&lt;&gt;$C$17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
+      <formula>$O$19&lt;&gt;$C$19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20">
     <cfRule type="expression" dxfId="21" priority="15">
-      <formula>$O$18&lt;&gt;$C$18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O20">
+      <formula>$O$20&lt;&gt;$C$20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22">
     <cfRule type="expression" dxfId="20" priority="14">
-      <formula>$O$20&lt;&gt;$C$20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O22">
+      <formula>$O$22&lt;&gt;$C$22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O24:O25">
     <cfRule type="expression" dxfId="19" priority="13">
-      <formula>$O$22&lt;&gt;$C$22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O24">
+      <formula>$O$24&lt;&gt;$C$24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27">
     <cfRule type="expression" dxfId="18" priority="12">
-      <formula>$O$24&lt;&gt;$C$24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O25">
+      <formula>$O$27&lt;&gt;$C$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28">
     <cfRule type="expression" dxfId="17" priority="11">
-      <formula>$O$25&lt;&gt;$C$25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O26">
+      <formula>$O$28&lt;&gt;$C$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O29">
     <cfRule type="expression" dxfId="16" priority="10">
-      <formula>$O$26&lt;&gt;$C$26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O27">
+      <formula>$O$29&lt;&gt;$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O30">
     <cfRule type="expression" dxfId="15" priority="9">
-      <formula>$O$27&lt;&gt;$C$27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O29">
+      <formula>$O$30&lt;&gt;$C$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O32">
     <cfRule type="expression" dxfId="14" priority="8">
-      <formula>$O$29&lt;&gt;$C$29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O30">
+      <formula>$O$32&lt;&gt;$C$32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O33">
     <cfRule type="expression" dxfId="13" priority="7">
-      <formula>$O$30&lt;&gt;$C$30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O32">
+      <formula>$O$33&lt;&gt;$C$33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O35">
     <cfRule type="expression" dxfId="12" priority="6">
-      <formula>$O$32&lt;&gt;$C$32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O34">
+      <formula>$O$35&lt;&gt;$C$35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O37">
     <cfRule type="expression" dxfId="11" priority="5">
-      <formula>$O$34&lt;&gt;$C$34</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O36">
+      <formula>$O$37&lt;&gt;$C$37</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O39">
     <cfRule type="expression" dxfId="10" priority="4">
-      <formula>$O$36&lt;&gt;$C$36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O38">
+      <formula>$O$39&lt;&gt;$C$39</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O41">
     <cfRule type="expression" dxfId="9" priority="3">
-      <formula>$O$38&lt;&gt;$C$38</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O40">
+      <formula>$O$41&lt;&gt;$C$41</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O43">
     <cfRule type="expression" dxfId="8" priority="2">
-      <formula>$O$40&lt;&gt;$C$40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O42">
+      <formula>$O$43&lt;&gt;$C$43</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O45">
     <cfRule type="expression" dxfId="7" priority="1">
-      <formula>$O$42&lt;&gt;$C$42</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O44">
+      <formula>$O$45&lt;&gt;$C$45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O47">
     <cfRule type="expression" dxfId="6" priority="25">
-      <formula>$O$44&lt;&gt;$C$44</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O45">
+      <formula>$O$47&lt;&gt;$C$47</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O48">
     <cfRule type="expression" dxfId="5" priority="24">
-      <formula>$O$45&lt;&gt;$C$45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O46">
+      <formula>$O$48&lt;&gt;$C$48</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O49">
     <cfRule type="expression" dxfId="4" priority="23">
-      <formula>$O$46&lt;&gt;$C$46</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O47">
+      <formula>$O$49&lt;&gt;$C$49</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O50">
     <cfRule type="expression" dxfId="3" priority="22">
-      <formula>$O$47&lt;&gt;$C$47</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O49">
+      <formula>$O$50&lt;&gt;$C$50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O52">
     <cfRule type="expression" dxfId="2" priority="31">
-      <formula>$O$49&lt;&gt;$C$49</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O50">
+      <formula>$O$52&lt;&gt;$C$52</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O53">
     <cfRule type="expression" dxfId="1" priority="32">
-      <formula xml:space="preserve"> $O$50&lt;&gt;$C$50</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O51">
+      <formula xml:space="preserve"> $O$53&lt;&gt;$C$53</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O54">
     <cfRule type="expression" dxfId="0" priority="33">
-      <formula xml:space="preserve"> $O$51&lt;&gt;$C$56</formula>
+      <formula xml:space="preserve"> $O$54&lt;&gt;$C$59</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="O4:O50" formulaRange="1"/>
+    <ignoredError sqref="O26:O53 O4:O9 O11:O13 O15:O24" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avancement de la doc technique
</commit_message>
<xml_diff>
--- a/docs/Planification.xlsx
+++ b/docs/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\var\www\Flavio_Soares_Rodrigues_TPI_2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA013641-FF6B-4ACD-A6C0-C9C8647C3E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD992B7-71F7-440C-9232-84B6BBCADC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>Page détails d'un article</t>
-  </si>
-  <si>
-    <t>Ajout au panier depuis la page de détails d'un article</t>
   </si>
   <si>
     <t>Temps
@@ -1020,465 +1017,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFBCFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="92">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -4354,10 +3893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AB6151-ACBB-4F8A-A877-2979D67AF922}">
-  <dimension ref="B1:P64"/>
+  <dimension ref="B1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -4376,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>1</v>
@@ -4412,7 +3951,7 @@
         <v>11</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -4539,7 +4078,9 @@
       <c r="E8" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -4550,7 +4091,7 @@
       <c r="N8" s="23"/>
       <c r="O8" s="9">
         <f t="shared" si="0"/>
-        <v>0.15625</v>
+        <v>0.16319444444444445</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4580,7 +4121,7 @@
     </row>
     <row r="10" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -4605,16 +4146,14 @@
     </row>
     <row r="11" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="7">
         <v>0.125</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -4625,7 +4164,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="34">
         <f>SUM(D11:N11)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4648,7 +4187,7 @@
     </row>
     <row r="13" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="7">
         <v>4.1666666666666664E-2</v>
@@ -4671,7 +4210,7 @@
     </row>
     <row r="14" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="24"/>
@@ -4689,7 +4228,7 @@
     </row>
     <row r="15" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="7">
         <v>2.7777777777777776E-2</v>
@@ -4799,7 +4338,7 @@
     </row>
     <row r="20" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="7">
         <v>1.3888888888888888E-2</v>
@@ -4881,7 +4420,7 @@
     </row>
     <row r="24" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="7">
         <v>4.1666666666666664E-2</v>
@@ -4904,7 +4443,7 @@
     </row>
     <row r="25" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
@@ -4942,7 +4481,7 @@
     </row>
     <row r="27" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="7">
         <v>2.7777777777777776E-2</v>
@@ -4965,7 +4504,7 @@
     </row>
     <row r="28" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="7">
         <v>1.3888888888888888E-2</v>
@@ -4988,7 +4527,7 @@
     </row>
     <row r="29" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7">
         <v>2.7777777777777776E-2</v>
@@ -5052,7 +4591,7 @@
     </row>
     <row r="32" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="7">
         <v>2.0833333333333332E-2</v>
@@ -5373,7 +4912,9 @@
       <c r="E47" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F47" s="4"/>
+      <c r="F47" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
@@ -5384,7 +4925,7 @@
       <c r="N47" s="23"/>
       <c r="O47" s="9">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>7.6388888888888881E-2</v>
       </c>
     </row>
     <row r="48" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5424,7 +4965,7 @@
         <v>0.125</v>
       </c>
       <c r="F49" s="4">
-        <v>8.3333333333333329E-2</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -5436,7 +4977,7 @@
       <c r="N49" s="23"/>
       <c r="O49" s="9">
         <f t="shared" si="0"/>
-        <v>0.2361111111111111</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="50" spans="2:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5544,7 +5085,7 @@
       </c>
       <c r="F54" s="5">
         <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="G54" s="5">
         <f t="shared" si="6"/>
@@ -5580,7 +5121,7 @@
       </c>
       <c r="O54" s="6">
         <f>SUM(D54:N54)</f>
-        <v>0.83333333333333337</v>
+        <v>0.83333333333333348</v>
       </c>
       <c r="P54" s="4"/>
     </row>
@@ -5721,11 +5262,6 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="E62:G62"/>

</xml_diff>